<commit_message>
Update: All Test and Pages
</commit_message>
<xml_diff>
--- a/src/test/java/com/saucedemo/TestData/testData.xlsx
+++ b/src/test/java/com/saucedemo/TestData/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huawe\eclipse-workspace\SauceDemo\src\test\java\com\saucedemo\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A665413E-8924-440E-BFE9-9A2436DC26D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEABC97-CE7C-4B44-92BA-50CBB3837A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>FirstName</t>
   </si>
@@ -42,18 +42,6 @@
     <t>Doe</t>
   </si>
   <si>
-    <t>Mary</t>
-  </si>
-  <si>
-    <t>Anne</t>
-  </si>
-  <si>
-    <t>Dan</t>
-  </si>
-  <si>
-    <t>Lui</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -66,15 +54,9 @@
     <t>secret_sauce</t>
   </si>
   <si>
-    <t>Test.allTheThings() T-Shirt (Red)</t>
-  </si>
-  <si>
     <t>Sauce Labs Backpack, Sauce Labs Bike Light, Sauce Labs Bolt T-Shirt</t>
   </si>
   <si>
-    <t>Sauce Labs Fleece Jacket, Sauce Labs Onesie</t>
-  </si>
-  <si>
     <t>AddProduct</t>
   </si>
   <si>
@@ -82,9 +64,6 @@
   </si>
   <si>
     <t>Sauce Labs Backpack</t>
-  </si>
-  <si>
-    <t>Sauce Labs Fleece Jacket</t>
   </si>
 </sst>
 </file>
@@ -414,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:AJ1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,10 +408,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -444,18 +423,18 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -467,56 +446,10 @@
         <v>54200</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1">
-        <v>53300</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1">
-        <v>48900</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>